<commit_message>
finalização dos links da movimentação
</commit_message>
<xml_diff>
--- a/layout telas chamadas.xlsx
+++ b/layout telas chamadas.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WorkSpacesCondominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C8660F9-EDD2-457C-849D-C83600534D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911B6C6B-B90E-45B8-A2DA-7ACAA3A4407B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="4" xr2:uid="{45BAC855-E0AE-4D66-8A26-B9192ACE72D6}"/>
+    <workbookView xWindow="30" yWindow="840" windowWidth="28800" windowHeight="11295" activeTab="3" xr2:uid="{45BAC855-E0AE-4D66-8A26-B9192ACE72D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
     <sheet name="listaCondominio" sheetId="2" r:id="rId2"/>
     <sheet name="Movimentação" sheetId="3" r:id="rId3"/>
-    <sheet name="calculos" sheetId="4" r:id="rId4"/>
+    <sheet name="Morador" sheetId="4" r:id="rId4"/>
     <sheet name="Contas" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F827065-EC61-4564-87F9-E2EC61747E05}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BAD5BF-F865-47E0-84C0-12BC4B21A7CB}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>